<commit_message>
added urls to desing pattersn
</commit_message>
<xml_diff>
--- a/Interview_questions.xlsx
+++ b/Interview_questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10686668\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10686668\Desktop\Interview\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74192A8A-1A75-4632-9491-6819445DBF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DFBADD-4A3F-41AC-B69B-C35DE241451E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="11" xr2:uid="{82056731-A5AD-406B-97C2-C69A7FA7A7BE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="8" xr2:uid="{82056731-A5AD-406B-97C2-C69A7FA7A7BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Coding" sheetId="8" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="120">
   <si>
     <t>semantic tags</t>
   </si>
@@ -396,6 +396,18 @@
   </si>
   <si>
     <t>Dynamic Programming</t>
+  </si>
+  <si>
+    <t>Meta tag</t>
+  </si>
+  <si>
+    <t>https://codewithpawan.medium.com/understanding-solid-principles-in-javascript-and-node-js-9abb09760049</t>
+  </si>
+  <si>
+    <t>https://www.freecodecamp.org/news/acid-databases-explained/</t>
+  </si>
+  <si>
+    <t>okta authentication</t>
   </si>
 </sst>
 </file>
@@ -773,7 +785,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -843,10 +855,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF6CE91-C21C-4C6B-9FC8-AE3F4F13FB9D}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -862,6 +874,11 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -916,33 +933,40 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B17FFC-8FBB-414A-9047-396323C9744A}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="91.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -990,7 +1014,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="46.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.08984375" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1111,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14703799-47C0-4E60-B06E-03F6B8E32554}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1252,15 +1276,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D178B9FA-B8CC-4EFB-B890-90262A85473E}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
@@ -1366,6 +1390,11 @@
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1507,7 +1536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EDC9E3-759C-4EA6-9A92-1E3B046C9F61}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
uploded JS Interview and DSA questions
</commit_message>
<xml_diff>
--- a/Interview_questions.xlsx
+++ b/Interview_questions.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10686668\Desktop\Interview\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DFBADD-4A3F-41AC-B69B-C35DE241451E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA27F48-FDEE-4E29-B073-384054A7FC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="8" xr2:uid="{82056731-A5AD-406B-97C2-C69A7FA7A7BE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{82056731-A5AD-406B-97C2-C69A7FA7A7BE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Coding" sheetId="8" r:id="rId1"/>
+    <sheet name="DSA" sheetId="8" r:id="rId1"/>
     <sheet name="Javascript" sheetId="1" r:id="rId2"/>
     <sheet name="Typescript" sheetId="14" r:id="rId3"/>
     <sheet name="Angular" sheetId="6" r:id="rId4"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
   <si>
     <t>semantic tags</t>
   </si>
@@ -408,6 +408,12 @@
   </si>
   <si>
     <t>okta authentication</t>
+  </si>
+  <si>
+    <t>1. Ways to create a deep clone, does destructing creats a deep clones</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1hXserPuxVoWMG9Hs7y8wVdRCJTcj3xMBAEYUOXQ5Xag/edit?usp=drivesdk</t>
   </si>
 </sst>
 </file>
@@ -782,68 +788,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A922EF1E-702D-4573-B051-F560392AE35E}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="97.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -1008,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98D25E3-39C4-42FD-AC41-D6180DAE3232}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1076,9 +1086,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -1111,10 +1124,13 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1278,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D178B9FA-B8CC-4EFB-B890-90262A85473E}">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1407,10 +1423,13 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1432,10 +1451,13 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1536,8 +1558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EDC9E3-759C-4EA6-9A92-1E3B046C9F61}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added zemoso technologies questions
</commit_message>
<xml_diff>
--- a/Interview_questions.xlsx
+++ b/Interview_questions.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10686668\Desktop\Interview\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA27F48-FDEE-4E29-B073-384054A7FC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960860F3-D756-4E97-A455-838AE24C5105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{82056731-A5AD-406B-97C2-C69A7FA7A7BE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{82056731-A5AD-406B-97C2-C69A7FA7A7BE}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA" sheetId="8" r:id="rId1"/>
-    <sheet name="Javascript" sheetId="1" r:id="rId2"/>
-    <sheet name="Typescript" sheetId="14" r:id="rId3"/>
-    <sheet name="Angular" sheetId="6" r:id="rId4"/>
-    <sheet name="nodejs" sheetId="2" r:id="rId5"/>
-    <sheet name="express" sheetId="3" r:id="rId6"/>
-    <sheet name="State Management" sheetId="12" r:id="rId7"/>
-    <sheet name="No SQL" sheetId="4" r:id="rId8"/>
-    <sheet name="SQL" sheetId="15" r:id="rId9"/>
-    <sheet name="HTML" sheetId="5" r:id="rId10"/>
-    <sheet name="CSS" sheetId="13" r:id="rId11"/>
-    <sheet name="Design Patterns" sheetId="11" r:id="rId12"/>
-    <sheet name="DevOps" sheetId="16" r:id="rId13"/>
+    <sheet name="MCQ" sheetId="17" r:id="rId2"/>
+    <sheet name="Javascript" sheetId="1" r:id="rId3"/>
+    <sheet name="Typescript" sheetId="14" r:id="rId4"/>
+    <sheet name="Angular" sheetId="6" r:id="rId5"/>
+    <sheet name="nodejs" sheetId="2" r:id="rId6"/>
+    <sheet name="express" sheetId="3" r:id="rId7"/>
+    <sheet name="State Management" sheetId="12" r:id="rId8"/>
+    <sheet name="No SQL" sheetId="4" r:id="rId9"/>
+    <sheet name="SQL" sheetId="15" r:id="rId10"/>
+    <sheet name="HTML" sheetId="5" r:id="rId11"/>
+    <sheet name="CSS" sheetId="13" r:id="rId12"/>
+    <sheet name="Design Patterns" sheetId="11" r:id="rId13"/>
+    <sheet name="DevOps" sheetId="16" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
   <si>
     <t>semantic tags</t>
   </si>
@@ -95,18 +96,12 @@
     <t>Encoding of data using base64</t>
   </si>
   <si>
-    <t>Find duplicates</t>
-  </si>
-  <si>
     <t>Web components</t>
   </si>
   <si>
     <t xml:space="preserve">Rest API Principals </t>
   </si>
   <si>
-    <t>Anagrams</t>
-  </si>
-  <si>
     <t>Sort, search, remove duplicates</t>
   </si>
   <si>
@@ -386,12 +381,6 @@
     <t>Url shortner</t>
   </si>
   <si>
-    <t>Print dynamic url or link using closures</t>
-  </si>
-  <si>
-    <t>Print prime using given range</t>
-  </si>
-  <si>
     <t>Matrix Problems</t>
   </si>
   <si>
@@ -414,6 +403,18 @@
   </si>
   <si>
     <t>https://docs.google.com/spreadsheets/d/1hXserPuxVoWMG9Hs7y8wVdRCJTcj3xMBAEYUOXQ5Xag/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>Not a Buffer.toString() encoding method</t>
+  </si>
+  <si>
+    <t>Purpose of Nodejs module system</t>
+  </si>
+  <si>
+    <t>How can async hooks be used to monito the lifecycle of asynchronous resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what is require keyword in nodejs </t>
   </si>
 </sst>
 </file>
@@ -788,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A922EF1E-702D-4573-B051-F560392AE35E}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -805,12 +806,12 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -820,42 +821,93 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EDC9E3-759C-4EA6-9A92-1E3B046C9F61}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="84.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -863,7 +915,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF6CE91-C21C-4C6B-9FC8-AE3F4F13FB9D}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -888,7 +940,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -896,7 +948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A4A006-6528-482B-9F24-E210DD8928C9}">
   <dimension ref="A1:A6"/>
   <sheetViews>
@@ -908,32 +960,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -941,7 +993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B17FFC-8FBB-414A-9047-396323C9744A}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -957,28 +1009,28 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -986,7 +1038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F575098-065A-43E3-81FF-21BD6A33AFCA}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1001,12 +1053,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1015,6 +1067,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C0EF7C-158B-407C-9C96-4481162D6933}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98D25E3-39C4-42FD-AC41-D6180DAE3232}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -1043,7 +1133,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1088,30 +1178,30 @@
     </row>
     <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1119,7 +1209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B04885-C7AE-46C6-9A3B-E50CA96E1344}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1134,12 +1224,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1147,7 +1237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14703799-47C0-4E60-B06E-03F6B8E32554}">
   <dimension ref="A1:A25"/>
   <sheetViews>
@@ -1167,122 +1257,122 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1290,11 +1380,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D178B9FA-B8CC-4EFB-B890-90262A85473E}">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -1305,112 +1395,112 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1418,7 +1508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7BA3978-13BD-48FB-8250-38D30D1B0F7B}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1433,12 +1523,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1446,7 +1536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC51E170-E5D2-4F10-8101-ACDCD1737390}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -1461,27 +1551,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1489,7 +1579,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB960A7-5B2E-4C75-AD12-58C2E87263C6}">
   <dimension ref="A1:A10"/>
   <sheetViews>
@@ -1501,127 +1591,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EDC9E3-759C-4EA6-9A92-1E3B046C9F61}">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="84.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
zemoso interview missed questions
</commit_message>
<xml_diff>
--- a/Interview_questions.xlsx
+++ b/Interview_questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10686668\Desktop\Interview\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53D0CF9-D604-42F9-9120-16D879F86E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC46AE7-C2D4-4BD7-BFB1-D87682ACA877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{82056731-A5AD-406B-97C2-C69A7FA7A7BE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="12" xr2:uid="{82056731-A5AD-406B-97C2-C69A7FA7A7BE}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA" sheetId="8" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="128">
   <si>
     <t>semantic tags</t>
   </si>
@@ -427,6 +427,12 @@
   </si>
   <si>
     <t>Handling Cors in nodejs</t>
+  </si>
+  <si>
+    <t>Difference between fork and spwan</t>
+  </si>
+  <si>
+    <t>CAP Therome</t>
   </si>
 </sst>
 </file>
@@ -1007,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B17FFC-8FBB-414A-9047-396323C9744A}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1043,6 +1049,11 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1394,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D178B9FA-B8CC-4EFB-B890-90262A85473E}">
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1533,6 +1544,11 @@
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
angular questions for tcs
</commit_message>
<xml_diff>
--- a/Interview_questions.xlsx
+++ b/Interview_questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10686668\Desktop\Interview\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7B7AE3-5D60-4B4A-BB7A-75F70ECF532B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF47D6B-2768-4846-9811-16588A36C975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="5" xr2:uid="{82056731-A5AD-406B-97C2-C69A7FA7A7BE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="4" xr2:uid="{82056731-A5AD-406B-97C2-C69A7FA7A7BE}"/>
   </bookViews>
   <sheets>
     <sheet name="DSA" sheetId="8" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="137">
   <si>
     <t>semantic tags</t>
   </si>
@@ -439,6 +439,27 @@
   </si>
   <si>
     <t>Text summirization</t>
+  </si>
+  <si>
+    <t>Decoraters</t>
+  </si>
+  <si>
+    <t>Directives</t>
+  </si>
+  <si>
+    <t>AOT and JIT</t>
+  </si>
+  <si>
+    <t>Types of Decoraters</t>
+  </si>
+  <si>
+    <t>custom decoraters</t>
+  </si>
+  <si>
+    <t>Unit testing in angular</t>
+  </si>
+  <si>
+    <t>Mocking api calls in angular for unit testing</t>
   </si>
 </sst>
 </file>
@@ -1268,15 +1289,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14703799-47C0-4E60-B06E-03F6B8E32554}">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
@@ -1402,6 +1423,46 @@
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1413,7 +1474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D178B9FA-B8CC-4EFB-B890-90262A85473E}">
   <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added questions by powerschool interview
</commit_message>
<xml_diff>
--- a/Interview_questions.xlsx
+++ b/Interview_questions.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10686668\Desktop\Interview\Interview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF47D6B-2768-4846-9811-16588A36C975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="4" xr2:uid="{82056731-A5AD-406B-97C2-C69A7FA7A7BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DSA" sheetId="8" r:id="rId1"/>
@@ -28,7 +27,7 @@
     <sheet name="Design Patterns" sheetId="11" r:id="rId13"/>
     <sheet name="DevOps" sheetId="16" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="159">
   <si>
     <t>semantic tags</t>
   </si>
@@ -72,9 +71,6 @@
     <t>Difference between arrow func and func</t>
   </si>
   <si>
-    <t>Polyfill for Promise.all</t>
-  </si>
-  <si>
     <t>Difference between Promise and Observable</t>
   </si>
   <si>
@@ -102,12 +98,6 @@
     <t xml:space="preserve">Rest API Principals </t>
   </si>
   <si>
-    <t>Sort, search, remove duplicates</t>
-  </si>
-  <si>
-    <t>Create array function polyfills</t>
-  </si>
-  <si>
     <t>Microfront ends</t>
   </si>
   <si>
@@ -378,12 +368,6 @@
     <t>With Operator in SQL</t>
   </si>
   <si>
-    <t>Url shortner</t>
-  </si>
-  <si>
-    <t>Matrix Problems</t>
-  </si>
-  <si>
     <t>Dynamic Programming</t>
   </si>
   <si>
@@ -405,9 +389,6 @@
     <t>https://docs.google.com/spreadsheets/d/1hXserPuxVoWMG9Hs7y8wVdRCJTcj3xMBAEYUOXQ5Xag/edit?usp=drivesdk</t>
   </si>
   <si>
-    <t>Not a Buffer.toString() encoding method</t>
-  </si>
-  <si>
     <t>Purpose of Nodejs module system</t>
   </si>
   <si>
@@ -460,13 +441,97 @@
   </si>
   <si>
     <t>Mocking api calls in angular for unit testing</t>
+  </si>
+  <si>
+    <t>Polyfills for Promise functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polyfills for array function </t>
+  </si>
+  <si>
+    <t>Two Pointer approach</t>
+  </si>
+  <si>
+    <t>Sliding Window Approach</t>
+  </si>
+  <si>
+    <t>Buffer.toString() encoding method</t>
+  </si>
+  <si>
+    <t>Why do we use rxjs</t>
+  </si>
+  <si>
+    <t>Can we use rxjs other than with http</t>
+  </si>
+  <si>
+    <t>Can we call api's without using rxjs in angular</t>
+  </si>
+  <si>
+    <t>Subject and Behavioural Subjects</t>
+  </si>
+  <si>
+    <t>Can we pass state between component using Ngrx which is done by subjects</t>
+  </si>
+  <si>
+    <t>Can we call http in  reducers</t>
+  </si>
+  <si>
+    <t>Selectors</t>
+  </si>
+  <si>
+    <t>Why cant we use localStorage to manage State instead of Ngrx</t>
+  </si>
+  <si>
+    <t>How do Components listens to data changes when there is a change in state using Ngrx</t>
+  </si>
+  <si>
+    <t>How to decide when to use Ngrx or RXJS</t>
+  </si>
+  <si>
+    <t>Any other ways to Manage state apart from Ngrx in Angular</t>
+  </si>
+  <si>
+    <t>How do we manage http calls in Ngrx</t>
+  </si>
+  <si>
+    <t>CDN Cache</t>
+  </si>
+  <si>
+    <t>TTL</t>
+  </si>
+  <si>
+    <t>CDN Purging</t>
+  </si>
+  <si>
+    <t>Performace Metrics of a web page</t>
+  </si>
+  <si>
+    <t>svg</t>
+  </si>
+  <si>
+    <t>canvas</t>
+  </si>
+  <si>
+    <t>String Buffer and String Builder and new String()</t>
+  </si>
+  <si>
+    <t>Mutable and Immutable</t>
+  </si>
+  <si>
+    <t>Steps to convert Monolithic to Microservices</t>
+  </si>
+  <si>
+    <t>How does Hasp Map internally works</t>
+  </si>
+  <si>
+    <t>Authentication with okta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -833,50 +898,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A922EF1E-702D-4573-B051-F560392AE35E}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="97.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="97.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -886,73 +946,73 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EDC9E3-759C-4EA6-9A92-1E3B046C9F61}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="84.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.08984375" customWidth="1"/>
+    <col min="1" max="1" width="84.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -961,31 +1021,41 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF6CE91-C21C-4C6B-9FC8-AE3F4F13FB9D}">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -994,43 +1064,43 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A4A006-6528-482B-9F24-E210DD8928C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1039,48 +1109,73 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B17FFC-8FBB-414A-9047-396323C9744A}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" customWidth="1"/>
-    <col min="2" max="2" width="91.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1089,26 +1184,26 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F575098-065A-43E3-81FF-21BD6A33AFCA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1117,36 +1212,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C0EF7C-158B-407C-9C96-4481162D6933}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1155,103 +1250,118 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98D25E3-39C4-42FD-AC41-D6180DAE3232}">
-  <dimension ref="A1:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="48.08984375" customWidth="1"/>
+    <col min="1" max="1" width="48.09765625" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="41.4">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>32</v>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1260,26 +1370,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B04885-C7AE-46C6-9A3B-E50CA96E1344}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1288,181 +1398,201 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14703799-47C0-4E60-B06E-03F6B8E32554}">
-  <dimension ref="A1:A33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="64.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1471,161 +1601,166 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D178B9FA-B8CC-4EFB-B890-90262A85473E}">
-  <dimension ref="A1:A29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="63.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>129</v>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1634,26 +1769,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7BA3978-13BD-48FB-8250-38D30D1B0F7B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="29.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1662,41 +1797,81 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC51E170-E5D2-4F10-8101-ACDCD1737390}">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="72.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>103</v>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1705,63 +1880,63 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB960A7-5B2E-4C75-AD12-58C2E87263C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>